<commit_message>
Release 2023-02-17 + templates
</commit_message>
<xml_diff>
--- a/server/pharmadex2/src/main/resources/static/shablon/TemplateExample.xlsx
+++ b/server/pharmadex2/src/main/resources/static/shablon/TemplateExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexk\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Irina\ПРОЭКТЫ\PDX\Мозамбик АдминСтруктура\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533DEBA2-6EDB-4D32-99C6-B9DADB5D8C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3307A8-1A4D-4280-BB3E-1C0C21BDC8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="264" windowWidth="20904" windowHeight="5928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10785" yWindow="1875" windowWidth="16935" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="11" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
   <si>
     <t>SN</t>
   </si>
@@ -166,13 +166,28 @@
   </si>
   <si>
     <t xml:space="preserve">République de Madagascar </t>
+  </si>
+  <si>
+    <t>zoom_province</t>
+  </si>
+  <si>
+    <t>zoom_district</t>
+  </si>
+  <si>
+    <t>zoom_community</t>
+  </si>
+  <si>
+    <t>zoom_country</t>
+  </si>
+  <si>
+    <t>zoom_communa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +368,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -535,7 +559,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -665,6 +689,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -746,7 +798,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="76" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,91 +807,101 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="76" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="76" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="78">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Accent3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Accent4 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Accent5 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20% - Accent6 2" xfId="73" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40% - Accent1 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Accent2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Accent3 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent4 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent5 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40% - Accent6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Accent1 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - Accent3 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Accent4 2" xfId="67" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Accent5 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60% - Accent6 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 2" xfId="68" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 2" xfId="72" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Bad 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Explanatory Text 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Good 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Heading 4 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
     <cellStyle name="Normal 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
     <cellStyle name="Normal 4" xfId="76" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Note 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Title 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Warning Text 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Гиперссылка" xfId="77" builtinId="8"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -883,9 +945,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -923,7 +985,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1029,7 +1091,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1179,23 +1241,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="11" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1211,11 +1275,26 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1223,14 +1302,29 @@
         <v>46</v>
       </c>
       <c r="E2" s="4">
-        <v>46.437980000000003</v>
+        <v>-18.5836708</v>
       </c>
       <c r="F2" s="4">
-        <v>-19.042176999999999</v>
+        <v>31.3113037</v>
+      </c>
+      <c r="G2" s="4">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>7</v>
+      </c>
+      <c r="I2" s="10">
+        <v>8</v>
+      </c>
+      <c r="J2" s="10">
+        <v>9</v>
+      </c>
+      <c r="K2" s="4">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I5" s="3"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1242,25 +1336,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" customWidth="1"/>
-    <col min="7" max="9" width="27.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="9" width="27.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1333,7 +1427,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1359,7 +1453,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1385,7 +1479,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1411,7 +1505,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1437,7 +1531,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1482,21 +1576,21 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1567,7 +1661,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1591,7 +1685,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1615,7 +1709,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1639,7 +1733,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1663,7 +1757,7 @@
         <v>-19.042176999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>